<commit_message>
Adding missing notes for new variables of metric files
</commit_message>
<xml_diff>
--- a/data/static_tables/metric_structure.xlsx
+++ b/data/static_tables/metric_structure.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\eGrid\production_model\users\russelle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\eGrid\production_model\users\russelle\egrid\data\static_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A77499-6EE8-4062-8C15-787FA8F9C63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B485BE9F-0D55-4169-A240-F001A6109FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UNT21" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6155" uniqueCount="2906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6165" uniqueCount="2906">
   <si>
     <t>Name</t>
   </si>
@@ -9682,7 +9682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
@@ -12962,8 +12962,8 @@
   <dimension ref="A1:IN248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -13140,7 +13140,9 @@
       <c r="D11" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="E11" s="144"/>
+      <c r="E11" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="59" t="s">
@@ -13170,7 +13172,9 @@
       <c r="D13" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="144"/>
+      <c r="E13" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="59" t="s">
@@ -16870,8 +16874,8 @@
   <dimension ref="A1:IN248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -17047,7 +17051,9 @@
       <c r="D11" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="E11" s="144"/>
+      <c r="E11" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="59" t="s">
@@ -17077,7 +17083,9 @@
       <c r="D13" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="144"/>
+      <c r="E13" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="59" t="s">
@@ -20778,7 +20786,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -20954,7 +20962,9 @@
       <c r="D11" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="E11" s="144"/>
+      <c r="E11" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="109" t="s">
@@ -20984,7 +20994,9 @@
       <c r="D13" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="144"/>
+      <c r="E13" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="109" t="s">
@@ -24685,7 +24697,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -24862,7 +24874,9 @@
       <c r="D11" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="E11" s="144"/>
+      <c r="E11" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="59" t="s">
@@ -24892,7 +24906,9 @@
       <c r="D13" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="144"/>
+      <c r="E13" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="59" t="s">
@@ -28593,7 +28609,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -28748,7 +28764,9 @@
       <c r="D9" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="E9" s="144"/>
+      <c r="E9" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="59" t="s">
@@ -28778,7 +28796,9 @@
       <c r="D11" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="E11" s="144"/>
+      <c r="E11" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="59" t="s">
@@ -32477,8 +32497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding missing 2 in new metric label
</commit_message>
<xml_diff>
--- a/data/static_tables/metric_structure.xlsx
+++ b/data/static_tables/metric_structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\eGrid\production_model\users\russelle\egrid\data\static_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B485BE9F-0D55-4169-A240-F001A6109FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A78D40C-E631-4B9D-9E13-4FC91691AD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6165" uniqueCount="2906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6165" uniqueCount="2907">
   <si>
     <t>Name</t>
   </si>
@@ -8775,6 +8775,9 @@
   </si>
   <si>
     <t>GGRSLOSS</t>
+  </si>
+  <si>
+    <t>DIRCTUSE2</t>
   </si>
 </sst>
 </file>
@@ -32499,7 +32502,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -32632,7 +32635,7 @@
         <v>2903</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>2902</v>
+        <v>2906</v>
       </c>
       <c r="C9" s="56" t="s">
         <v>34</v>
@@ -32666,6 +32669,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6c854b04-c9c6-4391-adbe-2e73191270e7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="059b9c67-646b-4b4e-9ab1-2b1c805d0390">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AD6200282E8E804DB7E47654D11346C2" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="334b3f607926cb22599f187b4c015ce1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="059b9c67-646b-4b4e-9ab1-2b1c805d0390" xmlns:ns3="c05e7bd6-26a7-41a1-805c-893279a3732f" xmlns:ns4="6c854b04-c9c6-4391-adbe-2e73191270e7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0fe548b9ff7492f3109b4e0b4a8efc8f" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="059b9c67-646b-4b4e-9ab1-2b1c805d0390"/>
@@ -32925,27 +32948,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6c854b04-c9c6-4391-adbe-2e73191270e7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="059b9c67-646b-4b4e-9ab1-2b1c805d0390">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCA6965B-A23A-4F60-9CAE-00FD555BD4D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A2EA77E-CA9B-4563-9A5E-2F50B3C8BA13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6c854b04-c9c6-4391-adbe-2e73191270e7"/>
+    <ds:schemaRef ds:uri="059b9c67-646b-4b4e-9ab1-2b1c805d0390"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FE51207-01AF-400E-9D05-58F426138751}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32963,23 +32985,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A2EA77E-CA9B-4563-9A5E-2F50B3C8BA13}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6c854b04-c9c6-4391-adbe-2e73191270e7"/>
-    <ds:schemaRef ds:uri="059b9c67-646b-4b4e-9ab1-2b1c805d0390"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCA6965B-A23A-4F60-9CAE-00FD555BD4D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding three missing rows to plant file structure - confirmed that this was an error in the file
</commit_message>
<xml_diff>
--- a/data/static_tables/metric_structure.xlsx
+++ b/data/static_tables/metric_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\eGrid\production_model\users\russelle\egrid\data\static_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A78D40C-E631-4B9D-9E13-4FC91691AD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3DB7BF-89D3-4A78-87EF-2D3443013D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UNT21" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6165" uniqueCount="2907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6177" uniqueCount="2913">
   <si>
     <t>Name</t>
   </si>
@@ -8778,6 +8778,24 @@
   </si>
   <si>
     <t>DIRCTUSE2</t>
+  </si>
+  <si>
+    <t>Plant annual CH4 input emission rate (kg/GJ)</t>
+  </si>
+  <si>
+    <t>Plant annual N2O input emission rate (kg/GJ)</t>
+  </si>
+  <si>
+    <t>Plant annual CO2 equivalent input emission rate (kg/GJ)</t>
+  </si>
+  <si>
+    <t>PLCH4RA</t>
+  </si>
+  <si>
+    <t>PLN2ORA</t>
+  </si>
+  <si>
+    <t>PLC2ERA</t>
   </si>
 </sst>
 </file>
@@ -10393,11 +10411,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:FQ173"/>
+  <dimension ref="A1:IN176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -11301,7 +11319,7 @@
       </c>
       <c r="E64" s="144"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:248" x14ac:dyDescent="0.2">
       <c r="A65" s="62" t="s">
         <v>225</v>
       </c>
@@ -11318,7 +11336,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:248" x14ac:dyDescent="0.2">
       <c r="A66" s="62" t="s">
         <v>227</v>
       </c>
@@ -11333,7 +11351,7 @@
       </c>
       <c r="E66" s="144"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:248" x14ac:dyDescent="0.2">
       <c r="A67" s="62" t="s">
         <v>229</v>
       </c>
@@ -11350,7 +11368,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:248" x14ac:dyDescent="0.2">
       <c r="A68" s="62" t="s">
         <v>231</v>
       </c>
@@ -11365,7 +11383,7 @@
       </c>
       <c r="E68" s="144"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:248" x14ac:dyDescent="0.2">
       <c r="A69" s="62" t="s">
         <v>233</v>
       </c>
@@ -11382,7 +11400,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:248" x14ac:dyDescent="0.2">
       <c r="A70" s="64" t="s">
         <v>235</v>
       </c>
@@ -11397,7 +11415,7 @@
       </c>
       <c r="E70" s="144"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:248" x14ac:dyDescent="0.2">
       <c r="A71" s="64" t="s">
         <v>238</v>
       </c>
@@ -11412,7 +11430,7 @@
       </c>
       <c r="E71" s="144"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:248" x14ac:dyDescent="0.2">
       <c r="A72" s="64" t="s">
         <v>240</v>
       </c>
@@ -11427,7 +11445,7 @@
       </c>
       <c r="E72" s="144"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:248" x14ac:dyDescent="0.2">
       <c r="A73" s="64" t="s">
         <v>242</v>
       </c>
@@ -11442,12 +11460,12 @@
       </c>
       <c r="E73" s="144"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:248" x14ac:dyDescent="0.2">
       <c r="A74" s="64" t="s">
-        <v>244</v>
-      </c>
-      <c r="B74" s="65" t="s">
-        <v>245</v>
+        <v>2907</v>
+      </c>
+      <c r="B74" s="17" t="s">
+        <v>2910</v>
       </c>
       <c r="C74" s="129" t="s">
         <v>206</v>
@@ -11456,314 +11474,935 @@
         <v>237</v>
       </c>
       <c r="E74" s="144"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="66" t="s">
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+      <c r="I74" s="10"/>
+      <c r="J74" s="10"/>
+      <c r="K74" s="10"/>
+      <c r="L74" s="10"/>
+      <c r="M74" s="10"/>
+      <c r="N74" s="10"/>
+      <c r="O74" s="10"/>
+      <c r="P74" s="10"/>
+      <c r="Q74" s="10"/>
+      <c r="R74" s="10"/>
+      <c r="S74" s="10"/>
+      <c r="T74" s="10"/>
+      <c r="U74" s="10"/>
+      <c r="V74" s="13"/>
+      <c r="W74" s="13"/>
+      <c r="X74" s="13"/>
+      <c r="Y74" s="13"/>
+      <c r="Z74" s="13"/>
+      <c r="AA74" s="13"/>
+      <c r="AB74" s="13"/>
+      <c r="AC74" s="13"/>
+      <c r="AD74" s="13"/>
+      <c r="AE74" s="13"/>
+      <c r="AF74" s="13"/>
+      <c r="AG74" s="13"/>
+      <c r="AH74" s="13"/>
+      <c r="AJ74" s="13"/>
+      <c r="AK74" s="13"/>
+      <c r="AL74" s="13"/>
+      <c r="AM74" s="13"/>
+      <c r="AN74" s="13"/>
+      <c r="AO74" s="13"/>
+      <c r="AP74" s="13"/>
+      <c r="AQ74" s="13"/>
+      <c r="AR74" s="13"/>
+      <c r="AS74" s="13"/>
+      <c r="AT74" s="13"/>
+      <c r="AU74" s="13"/>
+      <c r="AV74" s="13"/>
+      <c r="AW74" s="13"/>
+      <c r="AX74" s="13"/>
+      <c r="AY74" s="13"/>
+      <c r="AZ74" s="13"/>
+      <c r="BA74" s="13"/>
+      <c r="CK74" s="13"/>
+      <c r="CL74" s="13"/>
+      <c r="CM74" s="13"/>
+      <c r="CN74" s="13"/>
+      <c r="CO74" s="13"/>
+      <c r="CP74" s="12"/>
+      <c r="CQ74" s="12"/>
+      <c r="CR74" s="12"/>
+      <c r="CS74" s="12"/>
+      <c r="CT74" s="12"/>
+      <c r="CU74" s="12"/>
+      <c r="CV74" s="12"/>
+      <c r="CW74" s="12"/>
+      <c r="CX74" s="12"/>
+      <c r="CY74" s="12"/>
+      <c r="CZ74" s="12"/>
+      <c r="DA74" s="12"/>
+      <c r="DB74" s="12"/>
+      <c r="DC74" s="12"/>
+      <c r="DD74" s="12"/>
+      <c r="DE74" s="12"/>
+      <c r="DF74" s="13"/>
+      <c r="DG74" s="13"/>
+      <c r="DH74" s="13"/>
+      <c r="DI74" s="13"/>
+      <c r="DJ74" s="13"/>
+      <c r="DK74" s="13"/>
+      <c r="DL74" s="13"/>
+      <c r="DM74" s="13"/>
+      <c r="DN74" s="13"/>
+      <c r="DO74" s="13"/>
+      <c r="DP74" s="13"/>
+      <c r="DQ74" s="13"/>
+      <c r="DR74" s="13"/>
+      <c r="DS74" s="13"/>
+      <c r="DT74" s="13"/>
+      <c r="DU74" s="13"/>
+      <c r="DV74" s="13"/>
+      <c r="DW74" s="13"/>
+      <c r="DX74" s="13"/>
+      <c r="DY74" s="13"/>
+      <c r="DZ74" s="13"/>
+      <c r="EA74" s="13"/>
+      <c r="EB74" s="13"/>
+      <c r="EC74" s="13"/>
+      <c r="ED74" s="13"/>
+      <c r="EE74" s="13"/>
+      <c r="EF74" s="13"/>
+      <c r="EG74" s="13"/>
+      <c r="EH74" s="12"/>
+      <c r="EI74" s="12"/>
+      <c r="EJ74" s="12"/>
+      <c r="EK74" s="12"/>
+      <c r="EL74" s="12"/>
+      <c r="EM74" s="12"/>
+      <c r="EN74" s="12"/>
+      <c r="EO74" s="12"/>
+      <c r="EP74" s="13"/>
+      <c r="EQ74" s="13"/>
+      <c r="ER74" s="13"/>
+      <c r="ES74" s="13"/>
+      <c r="ET74" s="13"/>
+      <c r="EU74" s="13"/>
+      <c r="EV74" s="13"/>
+      <c r="EW74" s="13"/>
+      <c r="EX74" s="13"/>
+      <c r="EY74" s="13"/>
+      <c r="EZ74" s="13"/>
+      <c r="FA74" s="13"/>
+      <c r="FB74" s="13"/>
+      <c r="FC74" s="13"/>
+      <c r="FD74" s="13"/>
+      <c r="FE74" s="13"/>
+      <c r="FF74" s="13"/>
+      <c r="FG74" s="13"/>
+      <c r="FH74" s="13"/>
+      <c r="FI74" s="13"/>
+      <c r="FJ74" s="13"/>
+      <c r="FK74" s="13"/>
+      <c r="FL74" s="10"/>
+      <c r="FM74" s="10"/>
+      <c r="FN74" s="10"/>
+      <c r="FO74" s="10"/>
+      <c r="FP74" s="10"/>
+      <c r="FQ74" s="10"/>
+      <c r="FR74" s="10"/>
+      <c r="FS74" s="10"/>
+      <c r="FT74" s="10"/>
+      <c r="FU74" s="10"/>
+      <c r="FV74" s="10"/>
+      <c r="FW74" s="10"/>
+      <c r="FX74" s="10"/>
+      <c r="FY74" s="10"/>
+      <c r="FZ74" s="10"/>
+      <c r="GA74" s="10"/>
+      <c r="GB74" s="10"/>
+      <c r="GC74" s="10"/>
+      <c r="GD74" s="10"/>
+      <c r="GE74" s="10"/>
+      <c r="GF74" s="10"/>
+      <c r="GG74" s="10"/>
+      <c r="GH74" s="10"/>
+      <c r="GI74" s="10"/>
+      <c r="GJ74" s="10"/>
+      <c r="GK74" s="10"/>
+      <c r="GL74" s="10"/>
+      <c r="GM74" s="10"/>
+      <c r="GN74" s="10"/>
+      <c r="GO74" s="10"/>
+      <c r="GP74" s="10"/>
+      <c r="GQ74" s="10"/>
+      <c r="GR74" s="14"/>
+      <c r="GS74" s="14"/>
+      <c r="GT74" s="14"/>
+      <c r="GU74" s="14"/>
+      <c r="GV74" s="14"/>
+      <c r="GW74" s="14"/>
+      <c r="GX74" s="14"/>
+      <c r="GY74" s="14"/>
+      <c r="GZ74" s="14"/>
+      <c r="HA74" s="14"/>
+      <c r="HB74" s="14"/>
+      <c r="HC74" s="14"/>
+      <c r="HD74" s="14"/>
+      <c r="HE74" s="14"/>
+      <c r="HF74" s="14"/>
+      <c r="HG74" s="14"/>
+      <c r="HH74" s="10"/>
+      <c r="HI74" s="10"/>
+      <c r="HJ74" s="10"/>
+      <c r="HK74" s="10"/>
+      <c r="HL74" s="10"/>
+      <c r="HM74" s="10"/>
+      <c r="HN74" s="10"/>
+      <c r="HO74" s="10"/>
+      <c r="HP74" s="10"/>
+      <c r="HQ74" s="10"/>
+      <c r="HR74" s="10"/>
+      <c r="HS74" s="10"/>
+      <c r="HT74" s="10"/>
+      <c r="HU74" s="10"/>
+      <c r="HV74" s="10"/>
+      <c r="HW74" s="10"/>
+      <c r="HX74" s="10"/>
+      <c r="HY74" s="10"/>
+      <c r="HZ74" s="10"/>
+      <c r="IA74" s="10"/>
+      <c r="IB74" s="10"/>
+      <c r="IC74" s="10"/>
+      <c r="ID74" s="14"/>
+      <c r="IE74" s="14"/>
+      <c r="IF74" s="14"/>
+      <c r="IG74" s="14"/>
+      <c r="IH74" s="14"/>
+      <c r="II74" s="14"/>
+      <c r="IJ74" s="14"/>
+      <c r="IK74" s="14"/>
+      <c r="IL74" s="14"/>
+      <c r="IM74" s="14"/>
+      <c r="IN74" s="14"/>
+    </row>
+    <row r="75" spans="1:248" x14ac:dyDescent="0.2">
+      <c r="A75" s="64" t="s">
+        <v>2908</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>2911</v>
+      </c>
+      <c r="C75" s="129" t="s">
+        <v>206</v>
+      </c>
+      <c r="D75" s="129" t="s">
+        <v>237</v>
+      </c>
+      <c r="E75" s="144"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
+      <c r="J75" s="10"/>
+      <c r="K75" s="10"/>
+      <c r="L75" s="10"/>
+      <c r="M75" s="10"/>
+      <c r="N75" s="10"/>
+      <c r="O75" s="10"/>
+      <c r="P75" s="10"/>
+      <c r="Q75" s="10"/>
+      <c r="R75" s="10"/>
+      <c r="S75" s="10"/>
+      <c r="T75" s="10"/>
+      <c r="U75" s="10"/>
+      <c r="V75" s="13"/>
+      <c r="W75" s="13"/>
+      <c r="X75" s="13"/>
+      <c r="Y75" s="13"/>
+      <c r="Z75" s="13"/>
+      <c r="AA75" s="13"/>
+      <c r="AB75" s="13"/>
+      <c r="AC75" s="13"/>
+      <c r="AD75" s="13"/>
+      <c r="AE75" s="13"/>
+      <c r="AF75" s="13"/>
+      <c r="AG75" s="13"/>
+      <c r="AH75" s="13"/>
+      <c r="AJ75" s="13"/>
+      <c r="AK75" s="13"/>
+      <c r="AL75" s="13"/>
+      <c r="AM75" s="13"/>
+      <c r="AN75" s="13"/>
+      <c r="AO75" s="13"/>
+      <c r="AP75" s="13"/>
+      <c r="AQ75" s="13"/>
+      <c r="AR75" s="13"/>
+      <c r="AS75" s="13"/>
+      <c r="AT75" s="13"/>
+      <c r="AU75" s="13"/>
+      <c r="AV75" s="13"/>
+      <c r="AW75" s="13"/>
+      <c r="AX75" s="13"/>
+      <c r="AY75" s="13"/>
+      <c r="AZ75" s="13"/>
+      <c r="BA75" s="13"/>
+      <c r="CK75" s="13"/>
+      <c r="CL75" s="13"/>
+      <c r="CM75" s="13"/>
+      <c r="CN75" s="13"/>
+      <c r="CO75" s="13"/>
+      <c r="CP75" s="12"/>
+      <c r="CQ75" s="12"/>
+      <c r="CR75" s="12"/>
+      <c r="CS75" s="12"/>
+      <c r="CT75" s="12"/>
+      <c r="CU75" s="12"/>
+      <c r="CV75" s="12"/>
+      <c r="CW75" s="12"/>
+      <c r="CX75" s="12"/>
+      <c r="CY75" s="12"/>
+      <c r="CZ75" s="12"/>
+      <c r="DA75" s="12"/>
+      <c r="DB75" s="12"/>
+      <c r="DC75" s="12"/>
+      <c r="DD75" s="12"/>
+      <c r="DE75" s="12"/>
+      <c r="DF75" s="13"/>
+      <c r="DG75" s="13"/>
+      <c r="DH75" s="13"/>
+      <c r="DI75" s="13"/>
+      <c r="DJ75" s="13"/>
+      <c r="DK75" s="13"/>
+      <c r="DL75" s="13"/>
+      <c r="DM75" s="13"/>
+      <c r="DN75" s="13"/>
+      <c r="DO75" s="13"/>
+      <c r="DP75" s="13"/>
+      <c r="DQ75" s="13"/>
+      <c r="DR75" s="13"/>
+      <c r="DS75" s="13"/>
+      <c r="DT75" s="13"/>
+      <c r="DU75" s="13"/>
+      <c r="DV75" s="13"/>
+      <c r="DW75" s="13"/>
+      <c r="DX75" s="13"/>
+      <c r="DY75" s="13"/>
+      <c r="DZ75" s="13"/>
+      <c r="EA75" s="13"/>
+      <c r="EB75" s="13"/>
+      <c r="EC75" s="13"/>
+      <c r="ED75" s="13"/>
+      <c r="EE75" s="13"/>
+      <c r="EF75" s="13"/>
+      <c r="EG75" s="13"/>
+      <c r="EH75" s="12"/>
+      <c r="EI75" s="12"/>
+      <c r="EJ75" s="12"/>
+      <c r="EK75" s="12"/>
+      <c r="EL75" s="12"/>
+      <c r="EM75" s="12"/>
+      <c r="EN75" s="12"/>
+      <c r="EO75" s="12"/>
+      <c r="EP75" s="13"/>
+      <c r="EQ75" s="13"/>
+      <c r="ER75" s="13"/>
+      <c r="ES75" s="13"/>
+      <c r="ET75" s="13"/>
+      <c r="EU75" s="13"/>
+      <c r="EV75" s="13"/>
+      <c r="EW75" s="13"/>
+      <c r="EX75" s="13"/>
+      <c r="EY75" s="13"/>
+      <c r="EZ75" s="13"/>
+      <c r="FA75" s="13"/>
+      <c r="FB75" s="13"/>
+      <c r="FC75" s="13"/>
+      <c r="FD75" s="13"/>
+      <c r="FE75" s="13"/>
+      <c r="FF75" s="13"/>
+      <c r="FG75" s="13"/>
+      <c r="FH75" s="13"/>
+      <c r="FI75" s="13"/>
+      <c r="FJ75" s="13"/>
+      <c r="FK75" s="13"/>
+      <c r="FL75" s="10"/>
+      <c r="FM75" s="10"/>
+      <c r="FN75" s="10"/>
+      <c r="FO75" s="10"/>
+      <c r="FP75" s="10"/>
+      <c r="FQ75" s="10"/>
+      <c r="FR75" s="10"/>
+      <c r="FS75" s="10"/>
+      <c r="FT75" s="10"/>
+      <c r="FU75" s="10"/>
+      <c r="FV75" s="10"/>
+      <c r="FW75" s="10"/>
+      <c r="FX75" s="10"/>
+      <c r="FY75" s="10"/>
+      <c r="FZ75" s="10"/>
+      <c r="GA75" s="10"/>
+      <c r="GB75" s="10"/>
+      <c r="GC75" s="10"/>
+      <c r="GD75" s="10"/>
+      <c r="GE75" s="10"/>
+      <c r="GF75" s="10"/>
+      <c r="GG75" s="10"/>
+      <c r="GH75" s="10"/>
+      <c r="GI75" s="10"/>
+      <c r="GJ75" s="10"/>
+      <c r="GK75" s="10"/>
+      <c r="GL75" s="10"/>
+      <c r="GM75" s="10"/>
+      <c r="GN75" s="10"/>
+      <c r="GO75" s="10"/>
+      <c r="GP75" s="10"/>
+      <c r="GQ75" s="10"/>
+      <c r="GR75" s="14"/>
+      <c r="GS75" s="14"/>
+      <c r="GT75" s="14"/>
+      <c r="GU75" s="14"/>
+      <c r="GV75" s="14"/>
+      <c r="GW75" s="14"/>
+      <c r="GX75" s="14"/>
+      <c r="GY75" s="14"/>
+      <c r="GZ75" s="14"/>
+      <c r="HA75" s="14"/>
+      <c r="HB75" s="14"/>
+      <c r="HC75" s="14"/>
+      <c r="HD75" s="14"/>
+      <c r="HE75" s="14"/>
+      <c r="HF75" s="14"/>
+      <c r="HG75" s="14"/>
+      <c r="HH75" s="10"/>
+      <c r="HI75" s="10"/>
+      <c r="HJ75" s="10"/>
+      <c r="HK75" s="10"/>
+      <c r="HL75" s="10"/>
+      <c r="HM75" s="10"/>
+      <c r="HN75" s="10"/>
+      <c r="HO75" s="10"/>
+      <c r="HP75" s="10"/>
+      <c r="HQ75" s="10"/>
+      <c r="HR75" s="10"/>
+      <c r="HS75" s="10"/>
+      <c r="HT75" s="10"/>
+      <c r="HU75" s="10"/>
+      <c r="HV75" s="10"/>
+      <c r="HW75" s="10"/>
+      <c r="HX75" s="10"/>
+      <c r="HY75" s="10"/>
+      <c r="HZ75" s="10"/>
+      <c r="IA75" s="10"/>
+      <c r="IB75" s="10"/>
+      <c r="IC75" s="10"/>
+      <c r="ID75" s="14"/>
+      <c r="IE75" s="14"/>
+      <c r="IF75" s="14"/>
+      <c r="IG75" s="14"/>
+      <c r="IH75" s="14"/>
+      <c r="II75" s="14"/>
+      <c r="IJ75" s="14"/>
+      <c r="IK75" s="14"/>
+      <c r="IL75" s="14"/>
+      <c r="IM75" s="14"/>
+      <c r="IN75" s="14"/>
+    </row>
+    <row r="76" spans="1:248" x14ac:dyDescent="0.2">
+      <c r="A76" s="64" t="s">
+        <v>2909</v>
+      </c>
+      <c r="B76" s="17" t="s">
+        <v>2912</v>
+      </c>
+      <c r="C76" s="129" t="s">
+        <v>206</v>
+      </c>
+      <c r="D76" s="129" t="s">
+        <v>237</v>
+      </c>
+      <c r="E76" s="144"/>
+      <c r="F76" s="10"/>
+      <c r="G76" s="10"/>
+      <c r="H76" s="10"/>
+      <c r="I76" s="10"/>
+      <c r="J76" s="10"/>
+      <c r="K76" s="10"/>
+      <c r="L76" s="10"/>
+      <c r="M76" s="10"/>
+      <c r="N76" s="10"/>
+      <c r="O76" s="10"/>
+      <c r="P76" s="10"/>
+      <c r="Q76" s="10"/>
+      <c r="R76" s="10"/>
+      <c r="S76" s="10"/>
+      <c r="T76" s="10"/>
+      <c r="U76" s="10"/>
+      <c r="V76" s="13"/>
+      <c r="W76" s="13"/>
+      <c r="X76" s="13"/>
+      <c r="Y76" s="13"/>
+      <c r="Z76" s="13"/>
+      <c r="AA76" s="13"/>
+      <c r="AB76" s="13"/>
+      <c r="AC76" s="13"/>
+      <c r="AD76" s="13"/>
+      <c r="AE76" s="13"/>
+      <c r="AF76" s="13"/>
+      <c r="AG76" s="13"/>
+      <c r="AH76" s="13"/>
+      <c r="AJ76" s="13"/>
+      <c r="AK76" s="13"/>
+      <c r="AL76" s="13"/>
+      <c r="AM76" s="13"/>
+      <c r="AN76" s="13"/>
+      <c r="AO76" s="13"/>
+      <c r="AP76" s="13"/>
+      <c r="AQ76" s="13"/>
+      <c r="AR76" s="13"/>
+      <c r="AS76" s="13"/>
+      <c r="AT76" s="13"/>
+      <c r="AU76" s="13"/>
+      <c r="AV76" s="13"/>
+      <c r="AW76" s="13"/>
+      <c r="AX76" s="13"/>
+      <c r="AY76" s="13"/>
+      <c r="AZ76" s="13"/>
+      <c r="BA76" s="13"/>
+      <c r="CK76" s="13"/>
+      <c r="CL76" s="13"/>
+      <c r="CM76" s="13"/>
+      <c r="CN76" s="13"/>
+      <c r="CO76" s="13"/>
+      <c r="CP76" s="12"/>
+      <c r="CQ76" s="12"/>
+      <c r="CR76" s="12"/>
+      <c r="CS76" s="12"/>
+      <c r="CT76" s="12"/>
+      <c r="CU76" s="12"/>
+      <c r="CV76" s="12"/>
+      <c r="CW76" s="12"/>
+      <c r="CX76" s="12"/>
+      <c r="CY76" s="12"/>
+      <c r="CZ76" s="12"/>
+      <c r="DA76" s="12"/>
+      <c r="DB76" s="12"/>
+      <c r="DC76" s="12"/>
+      <c r="DD76" s="12"/>
+      <c r="DE76" s="12"/>
+      <c r="DF76" s="13"/>
+      <c r="DG76" s="13"/>
+      <c r="DH76" s="13"/>
+      <c r="DI76" s="13"/>
+      <c r="DJ76" s="13"/>
+      <c r="DK76" s="13"/>
+      <c r="DL76" s="13"/>
+      <c r="DM76" s="13"/>
+      <c r="DN76" s="13"/>
+      <c r="DO76" s="13"/>
+      <c r="DP76" s="13"/>
+      <c r="DQ76" s="13"/>
+      <c r="DR76" s="13"/>
+      <c r="DS76" s="13"/>
+      <c r="DT76" s="13"/>
+      <c r="DU76" s="13"/>
+      <c r="DV76" s="13"/>
+      <c r="DW76" s="13"/>
+      <c r="DX76" s="13"/>
+      <c r="DY76" s="13"/>
+      <c r="DZ76" s="13"/>
+      <c r="EA76" s="13"/>
+      <c r="EB76" s="13"/>
+      <c r="EC76" s="13"/>
+      <c r="ED76" s="13"/>
+      <c r="EE76" s="13"/>
+      <c r="EF76" s="13"/>
+      <c r="EG76" s="13"/>
+      <c r="EH76" s="12"/>
+      <c r="EI76" s="12"/>
+      <c r="EJ76" s="12"/>
+      <c r="EK76" s="12"/>
+      <c r="EL76" s="12"/>
+      <c r="EM76" s="12"/>
+      <c r="EN76" s="12"/>
+      <c r="EO76" s="12"/>
+      <c r="EP76" s="13"/>
+      <c r="EQ76" s="13"/>
+      <c r="ER76" s="13"/>
+      <c r="ES76" s="13"/>
+      <c r="ET76" s="13"/>
+      <c r="EU76" s="13"/>
+      <c r="EV76" s="13"/>
+      <c r="EW76" s="13"/>
+      <c r="EX76" s="13"/>
+      <c r="EY76" s="13"/>
+      <c r="EZ76" s="13"/>
+      <c r="FA76" s="13"/>
+      <c r="FB76" s="13"/>
+      <c r="FC76" s="13"/>
+      <c r="FD76" s="13"/>
+      <c r="FE76" s="13"/>
+      <c r="FF76" s="13"/>
+      <c r="FG76" s="13"/>
+      <c r="FH76" s="13"/>
+      <c r="FI76" s="13"/>
+      <c r="FJ76" s="13"/>
+      <c r="FK76" s="13"/>
+      <c r="FL76" s="10"/>
+      <c r="FM76" s="10"/>
+      <c r="FN76" s="10"/>
+      <c r="FO76" s="10"/>
+      <c r="FP76" s="10"/>
+      <c r="FQ76" s="10"/>
+      <c r="FR76" s="10"/>
+      <c r="FS76" s="10"/>
+      <c r="FT76" s="10"/>
+      <c r="FU76" s="10"/>
+      <c r="FV76" s="10"/>
+      <c r="FW76" s="10"/>
+      <c r="FX76" s="10"/>
+      <c r="FY76" s="10"/>
+      <c r="FZ76" s="10"/>
+      <c r="GA76" s="10"/>
+      <c r="GB76" s="10"/>
+      <c r="GC76" s="10"/>
+      <c r="GD76" s="10"/>
+      <c r="GE76" s="10"/>
+      <c r="GF76" s="10"/>
+      <c r="GG76" s="10"/>
+      <c r="GH76" s="10"/>
+      <c r="GI76" s="10"/>
+      <c r="GJ76" s="10"/>
+      <c r="GK76" s="10"/>
+      <c r="GL76" s="10"/>
+      <c r="GM76" s="10"/>
+      <c r="GN76" s="10"/>
+      <c r="GO76" s="10"/>
+      <c r="GP76" s="10"/>
+      <c r="GQ76" s="10"/>
+      <c r="GR76" s="14"/>
+      <c r="GS76" s="14"/>
+      <c r="GT76" s="14"/>
+      <c r="GU76" s="14"/>
+      <c r="GV76" s="14"/>
+      <c r="GW76" s="14"/>
+      <c r="GX76" s="14"/>
+      <c r="GY76" s="14"/>
+      <c r="GZ76" s="14"/>
+      <c r="HA76" s="14"/>
+      <c r="HB76" s="14"/>
+      <c r="HC76" s="14"/>
+      <c r="HD76" s="14"/>
+      <c r="HE76" s="14"/>
+      <c r="HF76" s="14"/>
+      <c r="HG76" s="14"/>
+      <c r="HH76" s="10"/>
+      <c r="HI76" s="10"/>
+      <c r="HJ76" s="10"/>
+      <c r="HK76" s="10"/>
+      <c r="HL76" s="10"/>
+      <c r="HM76" s="10"/>
+      <c r="HN76" s="10"/>
+      <c r="HO76" s="10"/>
+      <c r="HP76" s="10"/>
+      <c r="HQ76" s="10"/>
+      <c r="HR76" s="10"/>
+      <c r="HS76" s="10"/>
+      <c r="HT76" s="10"/>
+      <c r="HU76" s="10"/>
+      <c r="HV76" s="10"/>
+      <c r="HW76" s="10"/>
+      <c r="HX76" s="10"/>
+      <c r="HY76" s="10"/>
+      <c r="HZ76" s="10"/>
+      <c r="IA76" s="10"/>
+      <c r="IB76" s="10"/>
+      <c r="IC76" s="10"/>
+      <c r="ID76" s="14"/>
+      <c r="IE76" s="14"/>
+      <c r="IF76" s="14"/>
+      <c r="IG76" s="14"/>
+      <c r="IH76" s="14"/>
+      <c r="II76" s="14"/>
+      <c r="IJ76" s="14"/>
+      <c r="IK76" s="14"/>
+      <c r="IL76" s="14"/>
+      <c r="IM76" s="14"/>
+      <c r="IN76" s="14"/>
+    </row>
+    <row r="77" spans="1:248" x14ac:dyDescent="0.2">
+      <c r="A77" s="64" t="s">
+        <v>244</v>
+      </c>
+      <c r="B77" s="65" t="s">
+        <v>245</v>
+      </c>
+      <c r="C77" s="129" t="s">
+        <v>206</v>
+      </c>
+      <c r="D77" s="129" t="s">
+        <v>237</v>
+      </c>
+      <c r="E77" s="144"/>
+    </row>
+    <row r="78" spans="1:248" x14ac:dyDescent="0.2">
+      <c r="A78" s="66" t="s">
         <v>246</v>
       </c>
-      <c r="B75" s="67" t="s">
+      <c r="B78" s="67" t="s">
         <v>247</v>
       </c>
-      <c r="C75" s="149" t="s">
+      <c r="C78" s="149" t="s">
         <v>202</v>
       </c>
-      <c r="D75" s="149" t="s">
-        <v>203</v>
-      </c>
-      <c r="E75" s="144"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="66" t="s">
+      <c r="D78" s="149" t="s">
+        <v>203</v>
+      </c>
+      <c r="E78" s="144"/>
+    </row>
+    <row r="79" spans="1:248" x14ac:dyDescent="0.2">
+      <c r="A79" s="66" t="s">
         <v>248</v>
       </c>
-      <c r="B76" s="67" t="s">
+      <c r="B79" s="67" t="s">
         <v>249</v>
       </c>
-      <c r="C76" s="149" t="s">
-        <v>206</v>
-      </c>
-      <c r="D76" s="149" t="s">
-        <v>203</v>
-      </c>
-      <c r="E76" s="144" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="66" t="s">
+      <c r="C79" s="149" t="s">
+        <v>206</v>
+      </c>
+      <c r="D79" s="149" t="s">
+        <v>203</v>
+      </c>
+      <c r="E79" s="144" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="80" spans="1:248" x14ac:dyDescent="0.2">
+      <c r="A80" s="66" t="s">
         <v>250</v>
       </c>
-      <c r="B77" s="67" t="s">
+      <c r="B80" s="67" t="s">
         <v>251</v>
       </c>
-      <c r="C77" s="149" t="s">
+      <c r="C80" s="149" t="s">
         <v>202</v>
       </c>
-      <c r="D77" s="149" t="s">
-        <v>203</v>
-      </c>
-      <c r="E77" s="144"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="66" t="s">
-        <v>252</v>
-      </c>
-      <c r="B78" s="67" t="s">
-        <v>253</v>
-      </c>
-      <c r="C78" s="149" t="s">
-        <v>206</v>
-      </c>
-      <c r="D78" s="149" t="s">
-        <v>203</v>
-      </c>
-      <c r="E78" s="144" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="66" t="s">
-        <v>254</v>
-      </c>
-      <c r="B79" s="67" t="s">
-        <v>255</v>
-      </c>
-      <c r="C79" s="149" t="s">
-        <v>202</v>
-      </c>
-      <c r="D79" s="149" t="s">
-        <v>203</v>
-      </c>
-      <c r="E79" s="144"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="66" t="s">
-        <v>256</v>
-      </c>
-      <c r="B80" s="67" t="s">
-        <v>257</v>
-      </c>
-      <c r="C80" s="149" t="s">
-        <v>206</v>
-      </c>
       <c r="D80" s="149" t="s">
         <v>203</v>
       </c>
-      <c r="E80" s="144" t="s">
-        <v>179</v>
-      </c>
+      <c r="E80" s="144"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="66" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B81" s="67" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C81" s="149" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D81" s="149" t="s">
         <v>203</v>
       </c>
-      <c r="E81" s="144"/>
+      <c r="E81" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="66" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B82" s="67" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C82" s="149" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D82" s="149" t="s">
         <v>203</v>
       </c>
-      <c r="E82" s="144" t="s">
-        <v>179</v>
-      </c>
+      <c r="E82" s="144"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="66" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B83" s="67" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C83" s="149" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D83" s="149" t="s">
         <v>203</v>
       </c>
-      <c r="E83" s="144"/>
+      <c r="E83" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="66" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B84" s="67" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C84" s="149" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D84" s="149" t="s">
         <v>203</v>
       </c>
-      <c r="E84" s="144" t="s">
-        <v>179</v>
-      </c>
+      <c r="E84" s="144"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="66" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B85" s="67" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C85" s="149" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D85" s="149" t="s">
         <v>203</v>
       </c>
-      <c r="E85" s="144"/>
+      <c r="E85" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="66" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B86" s="67" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C86" s="149" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D86" s="149" t="s">
         <v>203</v>
       </c>
-      <c r="E86" s="144" t="s">
-        <v>179</v>
-      </c>
+      <c r="E86" s="144"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="66" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B87" s="67" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C87" s="149" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D87" s="149" t="s">
         <v>203</v>
       </c>
-      <c r="E87" s="144"/>
+      <c r="E87" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="66" t="s">
+        <v>266</v>
+      </c>
+      <c r="B88" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C88" s="149" t="s">
+        <v>202</v>
+      </c>
+      <c r="D88" s="149" t="s">
+        <v>203</v>
+      </c>
+      <c r="E88" s="144"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="66" t="s">
+        <v>268</v>
+      </c>
+      <c r="B89" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="C89" s="149" t="s">
+        <v>206</v>
+      </c>
+      <c r="D89" s="149" t="s">
+        <v>203</v>
+      </c>
+      <c r="E89" s="144" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="66" t="s">
+        <v>270</v>
+      </c>
+      <c r="B90" s="67" t="s">
+        <v>271</v>
+      </c>
+      <c r="C90" s="149" t="s">
+        <v>202</v>
+      </c>
+      <c r="D90" s="149" t="s">
+        <v>203</v>
+      </c>
+      <c r="E90" s="144"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="66" t="s">
         <v>272</v>
       </c>
-      <c r="B88" s="67" t="s">
+      <c r="B91" s="67" t="s">
         <v>273</v>
       </c>
-      <c r="C88" s="149" t="s">
-        <v>206</v>
-      </c>
-      <c r="D88" s="149" t="s">
-        <v>203</v>
-      </c>
-      <c r="E88" s="144" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" s="68" t="s">
+      <c r="C91" s="149" t="s">
+        <v>206</v>
+      </c>
+      <c r="D91" s="149" t="s">
+        <v>203</v>
+      </c>
+      <c r="E91" s="144" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="68" t="s">
         <v>274</v>
       </c>
-      <c r="B89" s="69" t="s">
+      <c r="B92" s="69" t="s">
         <v>275</v>
       </c>
-      <c r="C89" s="149" t="s">
+      <c r="C92" s="149" t="s">
         <v>202</v>
       </c>
-      <c r="D89" s="149" t="s">
-        <v>203</v>
-      </c>
-      <c r="E89" s="144"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" s="68" t="s">
+      <c r="D92" s="149" t="s">
+        <v>203</v>
+      </c>
+      <c r="E92" s="144"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="68" t="s">
         <v>276</v>
       </c>
-      <c r="B90" s="69" t="s">
+      <c r="B93" s="69" t="s">
         <v>277</v>
       </c>
-      <c r="C90" s="149" t="s">
-        <v>206</v>
-      </c>
-      <c r="D90" s="149" t="s">
-        <v>203</v>
-      </c>
-      <c r="E90" s="144" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" s="38" t="s">
-        <v>278</v>
-      </c>
-      <c r="B91" s="70" t="s">
-        <v>279</v>
-      </c>
-      <c r="C91" s="130" t="s">
-        <v>40</v>
-      </c>
-      <c r="D91" s="130" t="s">
-        <v>41</v>
-      </c>
-      <c r="E91" s="144"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="B92" s="70" t="s">
-        <v>281</v>
-      </c>
-      <c r="C92" s="130" t="s">
-        <v>40</v>
-      </c>
-      <c r="D92" s="130" t="s">
-        <v>41</v>
-      </c>
-      <c r="E92" s="144"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" s="38" t="s">
-        <v>282</v>
-      </c>
-      <c r="B93" s="70" t="s">
-        <v>283</v>
-      </c>
-      <c r="C93" s="130" t="s">
-        <v>40</v>
-      </c>
-      <c r="D93" s="130" t="s">
-        <v>41</v>
-      </c>
-      <c r="E93" s="144"/>
+      <c r="C93" s="149" t="s">
+        <v>206</v>
+      </c>
+      <c r="D93" s="149" t="s">
+        <v>203</v>
+      </c>
+      <c r="E93" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="38" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B94" s="70" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C94" s="130" t="s">
         <v>40</v>
@@ -11775,58 +12414,58 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="38" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B95" s="70" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C95" s="130" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D95" s="130" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E95" s="144"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="38" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B96" s="70" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C96" s="130" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D96" s="130" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E96" s="144"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="38" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B97" s="70" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C97" s="130" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D97" s="130" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E97" s="144"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="38" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B98" s="70" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C98" s="130" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D98" s="130" t="s">
         <v>51</v>
@@ -11835,88 +12474,100 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="38" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B99" s="70" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C99" s="130" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D99" s="130" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E99" s="144"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="38" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B100" s="70" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C100" s="130" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D100" s="130" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E100" s="144"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="38" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B101" s="70" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C101" s="130" t="s">
         <v>34</v>
       </c>
       <c r="D101" s="130" t="s">
+        <v>51</v>
+      </c>
+      <c r="E101" s="144"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="38" t="s">
+        <v>294</v>
+      </c>
+      <c r="B102" s="70" t="s">
+        <v>295</v>
+      </c>
+      <c r="C102" s="130" t="s">
+        <v>34</v>
+      </c>
+      <c r="D102" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="E101" s="144"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102" s="40" t="s">
-        <v>300</v>
-      </c>
-      <c r="B102" s="71" t="s">
-        <v>301</v>
-      </c>
-      <c r="C102" s="130"/>
-      <c r="D102" s="130"/>
       <c r="E102" s="144"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103" s="40" t="s">
-        <v>302</v>
-      </c>
-      <c r="B103" s="71" t="s">
-        <v>303</v>
-      </c>
-      <c r="C103" s="130"/>
-      <c r="D103" s="130"/>
+      <c r="A103" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="B103" s="70" t="s">
+        <v>297</v>
+      </c>
+      <c r="C103" s="130" t="s">
+        <v>34</v>
+      </c>
+      <c r="D103" s="130" t="s">
+        <v>35</v>
+      </c>
       <c r="E103" s="144"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A104" s="40" t="s">
-        <v>304</v>
-      </c>
-      <c r="B104" s="71" t="s">
-        <v>305</v>
-      </c>
-      <c r="C104" s="130"/>
-      <c r="D104" s="130"/>
+      <c r="A104" s="38" t="s">
+        <v>298</v>
+      </c>
+      <c r="B104" s="70" t="s">
+        <v>299</v>
+      </c>
+      <c r="C104" s="130" t="s">
+        <v>34</v>
+      </c>
+      <c r="D104" s="130" t="s">
+        <v>35</v>
+      </c>
       <c r="E104" s="144"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="40" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B105" s="71" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C105" s="130"/>
       <c r="D105" s="130"/>
@@ -11924,10 +12575,10 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="40" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B106" s="71" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="C106" s="130"/>
       <c r="D106" s="130"/>
@@ -11935,10 +12586,10 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="40" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B107" s="71" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C107" s="130"/>
       <c r="D107" s="130"/>
@@ -11946,10 +12597,10 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="40" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="B108" s="71" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C108" s="130"/>
       <c r="D108" s="130"/>
@@ -11957,10 +12608,10 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="40" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B109" s="71" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C109" s="130"/>
       <c r="D109" s="130"/>
@@ -11968,66 +12619,54 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="40" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B110" s="71" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C110" s="130"/>
       <c r="D110" s="130"/>
       <c r="E110" s="144"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111" s="72" t="s">
-        <v>318</v>
-      </c>
-      <c r="B111" s="73" t="s">
-        <v>319</v>
-      </c>
-      <c r="C111" s="131" t="s">
-        <v>40</v>
-      </c>
-      <c r="D111" s="131" t="s">
-        <v>41</v>
-      </c>
+      <c r="A111" s="40" t="s">
+        <v>312</v>
+      </c>
+      <c r="B111" s="71" t="s">
+        <v>313</v>
+      </c>
+      <c r="C111" s="130"/>
+      <c r="D111" s="130"/>
       <c r="E111" s="144"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A112" s="72" t="s">
-        <v>320</v>
-      </c>
-      <c r="B112" s="73" t="s">
-        <v>321</v>
-      </c>
-      <c r="C112" s="131" t="s">
-        <v>40</v>
-      </c>
-      <c r="D112" s="131" t="s">
-        <v>41</v>
-      </c>
+      <c r="A112" s="40" t="s">
+        <v>314</v>
+      </c>
+      <c r="B112" s="71" t="s">
+        <v>315</v>
+      </c>
+      <c r="C112" s="130"/>
+      <c r="D112" s="130"/>
       <c r="E112" s="144"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A113" s="72" t="s">
-        <v>322</v>
-      </c>
-      <c r="B113" s="73" t="s">
-        <v>323</v>
-      </c>
-      <c r="C113" s="131" t="s">
-        <v>40</v>
-      </c>
-      <c r="D113" s="131" t="s">
-        <v>41</v>
-      </c>
+      <c r="A113" s="40" t="s">
+        <v>316</v>
+      </c>
+      <c r="B113" s="71" t="s">
+        <v>317</v>
+      </c>
+      <c r="C113" s="130"/>
+      <c r="D113" s="130"/>
       <c r="E113" s="144"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="72" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B114" s="73" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="C114" s="131" t="s">
         <v>40</v>
@@ -12039,115 +12678,115 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="72" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B115" s="73" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C115" s="131" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D115" s="131" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E115" s="144"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="72" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="B116" s="73" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C116" s="131" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D116" s="131" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E116" s="144"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="72" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="B117" s="73" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C117" s="131" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D117" s="131" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E117" s="144"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="72" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="B118" s="73" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="C118" s="131" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D118" s="131" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E118" s="144"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="72" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="B119" s="73" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C119" s="131" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D119" s="131" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E119" s="144"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="72" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B120" s="73" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C120" s="131" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D120" s="131" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E120" s="144"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="72" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="B121" s="73" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C121" s="131" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D121" s="131" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E121" s="144"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="72" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="B122" s="73" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C122" s="131" t="s">
         <v>40</v>
@@ -12159,612 +12798,612 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="72" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B123" s="73" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C123" s="131" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D123" s="131" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E123" s="144"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="72" t="s">
+        <v>338</v>
+      </c>
+      <c r="B124" s="73" t="s">
+        <v>339</v>
+      </c>
+      <c r="C124" s="131" t="s">
+        <v>40</v>
+      </c>
+      <c r="D124" s="131" t="s">
+        <v>41</v>
+      </c>
+      <c r="E124" s="144"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" s="72" t="s">
+        <v>340</v>
+      </c>
+      <c r="B125" s="73" t="s">
+        <v>341</v>
+      </c>
+      <c r="C125" s="131" t="s">
+        <v>40</v>
+      </c>
+      <c r="D125" s="131" t="s">
+        <v>41</v>
+      </c>
+      <c r="E125" s="144"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" s="72" t="s">
+        <v>342</v>
+      </c>
+      <c r="B126" s="73" t="s">
+        <v>343</v>
+      </c>
+      <c r="C126" s="131" t="s">
+        <v>50</v>
+      </c>
+      <c r="D126" s="131" t="s">
+        <v>51</v>
+      </c>
+      <c r="E126" s="144"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" s="72" t="s">
         <v>344</v>
       </c>
-      <c r="B124" s="73" t="s">
+      <c r="B127" s="73" t="s">
         <v>345</v>
       </c>
-      <c r="C124" s="131" t="s">
+      <c r="C127" s="131" t="s">
         <v>50</v>
       </c>
-      <c r="D124" s="131" t="s">
+      <c r="D127" s="131" t="s">
         <v>51</v>
       </c>
-      <c r="E124" s="144"/>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A125" s="74" t="s">
+      <c r="E127" s="144"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" s="74" t="s">
         <v>346</v>
       </c>
-      <c r="B125" s="50" t="s">
+      <c r="B128" s="50" t="s">
         <v>347</v>
       </c>
-      <c r="C125" s="122" t="s">
+      <c r="C128" s="122" t="s">
         <v>348</v>
       </c>
-      <c r="D125" s="122" t="s">
+      <c r="D128" s="122" t="s">
         <v>348</v>
-      </c>
-      <c r="E125" s="144"/>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A126" s="75" t="s">
-        <v>349</v>
-      </c>
-      <c r="B126" s="76" t="s">
-        <v>350</v>
-      </c>
-      <c r="C126" s="76" t="s">
-        <v>93</v>
-      </c>
-      <c r="D126" s="76" t="s">
-        <v>93</v>
-      </c>
-      <c r="E126" s="144"/>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A127" s="75" t="s">
-        <v>351</v>
-      </c>
-      <c r="B127" s="76" t="s">
-        <v>352</v>
-      </c>
-      <c r="C127" s="76" t="s">
-        <v>34</v>
-      </c>
-      <c r="D127" s="76" t="s">
-        <v>93</v>
-      </c>
-      <c r="E127" s="144" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A128" s="75" t="s">
-        <v>353</v>
-      </c>
-      <c r="B128" s="76" t="s">
-        <v>354</v>
-      </c>
-      <c r="C128" s="76" t="s">
-        <v>93</v>
-      </c>
-      <c r="D128" s="76" t="s">
-        <v>93</v>
       </c>
       <c r="E128" s="144"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="75" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B129" s="76" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C129" s="76" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="D129" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E129" s="144" t="s">
-        <v>179</v>
-      </c>
+      <c r="E129" s="144"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="75" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B130" s="76" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="C130" s="76" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="D130" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E130" s="144"/>
+      <c r="E130" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="75" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="B131" s="76" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="C131" s="76" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="D131" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E131" s="144" t="s">
-        <v>179</v>
-      </c>
+      <c r="E131" s="144"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="75" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="B132" s="76" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C132" s="76" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="D132" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E132" s="144"/>
+      <c r="E132" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="75" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="B133" s="76" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C133" s="76" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="D133" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E133" s="144" t="s">
-        <v>179</v>
-      </c>
+      <c r="E133" s="144"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="75" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="B134" s="76" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C134" s="76" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="D134" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E134" s="144"/>
+      <c r="E134" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="75" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="B135" s="76" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="C135" s="76" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="D135" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E135" s="144" t="s">
-        <v>179</v>
-      </c>
+      <c r="E135" s="144"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="75" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="B136" s="76" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C136" s="76" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="D136" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E136" s="144"/>
+      <c r="E136" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="75" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B137" s="76" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C137" s="76" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="D137" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E137" s="144" t="s">
-        <v>179</v>
-      </c>
+      <c r="E137" s="144"/>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="75" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B138" s="76" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C138" s="76" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="D138" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E138" s="144"/>
+      <c r="E138" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="75" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="B139" s="76" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="C139" s="76" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="D139" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E139" s="144" t="s">
-        <v>179</v>
-      </c>
+      <c r="E139" s="144"/>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="75" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="B140" s="76" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="C140" s="76" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="D140" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E140" s="144"/>
+      <c r="E140" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="75" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="B141" s="76" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C141" s="76" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="D141" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E141" s="144" t="s">
-        <v>179</v>
-      </c>
+      <c r="E141" s="144"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="75" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B142" s="76" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="C142" s="76" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="D142" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E142" s="144"/>
+      <c r="E142" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="75" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="B143" s="76" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="C143" s="76" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="D143" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E143" s="144" t="s">
-        <v>179</v>
-      </c>
+      <c r="E143" s="144"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="75" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="B144" s="76" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="C144" s="76" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="D144" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E144" s="144"/>
+      <c r="E144" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="75" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="B145" s="76" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="C145" s="76" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="D145" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E145" s="144" t="s">
-        <v>179</v>
-      </c>
+      <c r="E145" s="144"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="75" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="B146" s="76" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="C146" s="76" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="D146" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="E146" s="144"/>
+      <c r="E146" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="75" t="s">
+        <v>385</v>
+      </c>
+      <c r="B147" s="76" t="s">
+        <v>386</v>
+      </c>
+      <c r="C147" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="D147" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="E147" s="144"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" s="75" t="s">
+        <v>387</v>
+      </c>
+      <c r="B148" s="76" t="s">
+        <v>388</v>
+      </c>
+      <c r="C148" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="D148" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="E148" s="144" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" s="75" t="s">
+        <v>389</v>
+      </c>
+      <c r="B149" s="76" t="s">
+        <v>390</v>
+      </c>
+      <c r="C149" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="D149" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="E149" s="144"/>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" s="75" t="s">
         <v>391</v>
       </c>
-      <c r="B147" s="76" t="s">
+      <c r="B150" s="76" t="s">
         <v>392</v>
       </c>
-      <c r="C147" s="76" t="s">
+      <c r="C150" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="D147" s="76" t="s">
-        <v>93</v>
-      </c>
-      <c r="E147" s="144" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A148" s="77" t="s">
-        <v>393</v>
-      </c>
-      <c r="B148" s="78" t="s">
-        <v>394</v>
-      </c>
-      <c r="C148" s="78" t="s">
-        <v>93</v>
-      </c>
-      <c r="D148" s="78" t="s">
-        <v>93</v>
-      </c>
-      <c r="E148" s="144"/>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A149" s="77" t="s">
-        <v>395</v>
-      </c>
-      <c r="B149" s="78" t="s">
-        <v>396</v>
-      </c>
-      <c r="C149" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="D149" s="78" t="s">
-        <v>93</v>
-      </c>
-      <c r="E149" s="144" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A150" s="77" t="s">
-        <v>397</v>
-      </c>
-      <c r="B150" s="78" t="s">
-        <v>398</v>
-      </c>
-      <c r="C150" s="78" t="s">
-        <v>93</v>
-      </c>
-      <c r="D150" s="78" t="s">
-        <v>93</v>
-      </c>
-      <c r="E150" s="144"/>
+      <c r="D150" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="E150" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="77" t="s">
+        <v>393</v>
+      </c>
+      <c r="B151" s="78" t="s">
+        <v>394</v>
+      </c>
+      <c r="C151" s="78" t="s">
+        <v>93</v>
+      </c>
+      <c r="D151" s="78" t="s">
+        <v>93</v>
+      </c>
+      <c r="E151" s="144"/>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" s="77" t="s">
+        <v>395</v>
+      </c>
+      <c r="B152" s="78" t="s">
+        <v>396</v>
+      </c>
+      <c r="C152" s="78" t="s">
+        <v>34</v>
+      </c>
+      <c r="D152" s="78" t="s">
+        <v>93</v>
+      </c>
+      <c r="E152" s="144" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" s="77" t="s">
+        <v>397</v>
+      </c>
+      <c r="B153" s="78" t="s">
+        <v>398</v>
+      </c>
+      <c r="C153" s="78" t="s">
+        <v>93</v>
+      </c>
+      <c r="D153" s="78" t="s">
+        <v>93</v>
+      </c>
+      <c r="E153" s="144"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" s="77" t="s">
         <v>399</v>
       </c>
-      <c r="B151" s="78" t="s">
+      <c r="B154" s="78" t="s">
         <v>400</v>
       </c>
-      <c r="C151" s="78" t="s">
+      <c r="C154" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="D151" s="78" t="s">
-        <v>93</v>
-      </c>
-      <c r="E151" s="144" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A152" s="79" t="s">
+      <c r="D154" s="78" t="s">
+        <v>93</v>
+      </c>
+      <c r="E154" s="144" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" s="79" t="s">
         <v>401</v>
       </c>
-      <c r="B152" s="80" t="s">
+      <c r="B155" s="80" t="s">
         <v>402</v>
       </c>
-      <c r="C152" s="80" t="s">
-        <v>93</v>
-      </c>
-      <c r="D152" s="80" t="s">
-        <v>93</v>
-      </c>
-      <c r="E152" s="144"/>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A153" s="79" t="s">
+      <c r="C155" s="80" t="s">
+        <v>93</v>
+      </c>
+      <c r="D155" s="80" t="s">
+        <v>93</v>
+      </c>
+      <c r="E155" s="144"/>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" s="79" t="s">
         <v>403</v>
       </c>
-      <c r="B153" s="80" t="s">
+      <c r="B156" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="C153" s="80" t="s">
+      <c r="C156" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="D153" s="80" t="s">
-        <v>93</v>
-      </c>
-      <c r="E153" s="144" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A154" s="81" t="s">
-        <v>405</v>
-      </c>
-      <c r="B154" s="82" t="s">
-        <v>406</v>
-      </c>
-      <c r="C154" s="148" t="s">
-        <v>93</v>
-      </c>
-      <c r="D154" s="148" t="s">
-        <v>93</v>
-      </c>
-      <c r="E154" s="144"/>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A155" s="81" t="s">
-        <v>407</v>
-      </c>
-      <c r="B155" s="82" t="s">
-        <v>408</v>
-      </c>
-      <c r="C155" s="148" t="s">
-        <v>34</v>
-      </c>
-      <c r="D155" s="148" t="s">
-        <v>93</v>
-      </c>
-      <c r="E155" s="144" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A156" s="81" t="s">
-        <v>409</v>
-      </c>
-      <c r="B156" s="82" t="s">
-        <v>410</v>
-      </c>
-      <c r="C156" s="148" t="s">
-        <v>93</v>
-      </c>
-      <c r="D156" s="148" t="s">
-        <v>93</v>
-      </c>
-      <c r="E156" s="144"/>
+      <c r="D156" s="80" t="s">
+        <v>93</v>
+      </c>
+      <c r="E156" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="81" t="s">
+        <v>405</v>
+      </c>
+      <c r="B157" s="82" t="s">
+        <v>406</v>
+      </c>
+      <c r="C157" s="148" t="s">
+        <v>93</v>
+      </c>
+      <c r="D157" s="148" t="s">
+        <v>93</v>
+      </c>
+      <c r="E157" s="144"/>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" s="81" t="s">
+        <v>407</v>
+      </c>
+      <c r="B158" s="82" t="s">
+        <v>408</v>
+      </c>
+      <c r="C158" s="148" t="s">
+        <v>34</v>
+      </c>
+      <c r="D158" s="148" t="s">
+        <v>93</v>
+      </c>
+      <c r="E158" s="144" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" s="81" t="s">
+        <v>409</v>
+      </c>
+      <c r="B159" s="82" t="s">
+        <v>410</v>
+      </c>
+      <c r="C159" s="148" t="s">
+        <v>93</v>
+      </c>
+      <c r="D159" s="148" t="s">
+        <v>93</v>
+      </c>
+      <c r="E159" s="144"/>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" s="81" t="s">
         <v>411</v>
       </c>
-      <c r="B157" s="82" t="s">
+      <c r="B160" s="82" t="s">
         <v>412</v>
       </c>
-      <c r="C157" s="148" t="s">
+      <c r="C160" s="148" t="s">
         <v>34</v>
       </c>
-      <c r="D157" s="148" t="s">
-        <v>93</v>
-      </c>
-      <c r="E157" s="144" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A158" s="83" t="s">
-        <v>413</v>
-      </c>
-      <c r="B158" s="84" t="s">
-        <v>414</v>
-      </c>
-      <c r="C158" s="132" t="s">
-        <v>415</v>
-      </c>
-      <c r="D158" s="132" t="s">
-        <v>415</v>
-      </c>
-      <c r="E158" s="144"/>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A159" s="83" t="s">
-        <v>416</v>
-      </c>
-      <c r="B159" s="84" t="s">
-        <v>417</v>
-      </c>
-      <c r="C159" s="132" t="s">
-        <v>415</v>
-      </c>
-      <c r="D159" s="132" t="s">
-        <v>415</v>
-      </c>
-      <c r="E159" s="144"/>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A160" s="83" t="s">
-        <v>418</v>
-      </c>
-      <c r="B160" s="84" t="s">
-        <v>419</v>
-      </c>
-      <c r="C160" s="132" t="s">
-        <v>415</v>
-      </c>
-      <c r="D160" s="132" t="s">
-        <v>415</v>
-      </c>
-      <c r="E160" s="144"/>
+      <c r="D160" s="148" t="s">
+        <v>93</v>
+      </c>
+      <c r="E160" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="83" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="B161" s="84" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="C161" s="132" t="s">
         <v>415</v>
@@ -12776,10 +13415,10 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="83" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="B162" s="84" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="C162" s="132" t="s">
         <v>415</v>
@@ -12791,10 +13430,10 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="83" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="B163" s="84" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="C163" s="132" t="s">
         <v>415</v>
@@ -12806,10 +13445,10 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="83" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="B164" s="84" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="C164" s="132" t="s">
         <v>415</v>
@@ -12821,10 +13460,10 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="83" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="B165" s="84" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="C165" s="132" t="s">
         <v>415</v>
@@ -12836,10 +13475,10 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="83" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="B166" s="84" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="C166" s="132" t="s">
         <v>415</v>
@@ -12851,10 +13490,10 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="83" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="B167" s="84" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="C167" s="132" t="s">
         <v>415</v>
@@ -12866,10 +13505,10 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="83" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="B168" s="84" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="C168" s="132" t="s">
         <v>415</v>
@@ -12880,79 +13519,124 @@
       <c r="E168" s="144"/>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A169" s="85" t="s">
+      <c r="A169" s="83" t="s">
+        <v>430</v>
+      </c>
+      <c r="B169" s="84" t="s">
+        <v>431</v>
+      </c>
+      <c r="C169" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="D169" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="E169" s="144"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170" s="83" t="s">
+        <v>432</v>
+      </c>
+      <c r="B170" s="84" t="s">
+        <v>433</v>
+      </c>
+      <c r="C170" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="D170" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="E170" s="144"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171" s="83" t="s">
+        <v>434</v>
+      </c>
+      <c r="B171" s="84" t="s">
+        <v>435</v>
+      </c>
+      <c r="C171" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="D171" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="E171" s="144"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172" s="85" t="s">
         <v>436</v>
       </c>
-      <c r="B169" s="86" t="s">
+      <c r="B172" s="86" t="s">
         <v>437</v>
       </c>
-      <c r="C169" s="133" t="s">
+      <c r="C172" s="133" t="s">
         <v>415</v>
       </c>
-      <c r="D169" s="133" t="s">
+      <c r="D172" s="133" t="s">
         <v>415</v>
       </c>
-      <c r="E169" s="144"/>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A170" s="85" t="s">
+      <c r="E172" s="144"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173" s="85" t="s">
         <v>438</v>
       </c>
-      <c r="B170" s="86" t="s">
+      <c r="B173" s="86" t="s">
         <v>439</v>
       </c>
-      <c r="C170" s="133" t="s">
+      <c r="C173" s="133" t="s">
         <v>415</v>
       </c>
-      <c r="D170" s="133" t="s">
+      <c r="D173" s="133" t="s">
         <v>415</v>
       </c>
-      <c r="E170" s="144"/>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A171" s="87" t="s">
+      <c r="E173" s="144"/>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174" s="87" t="s">
         <v>440</v>
       </c>
-      <c r="B171" s="88" t="s">
+      <c r="B174" s="88" t="s">
         <v>441</v>
       </c>
-      <c r="C171" s="134" t="s">
+      <c r="C174" s="134" t="s">
         <v>415</v>
       </c>
-      <c r="D171" s="134" t="s">
+      <c r="D174" s="134" t="s">
         <v>415</v>
       </c>
-      <c r="E171" s="144"/>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A172" s="89" t="s">
+      <c r="E174" s="144"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175" s="89" t="s">
         <v>442</v>
       </c>
-      <c r="B172" s="90" t="s">
+      <c r="B175" s="90" t="s">
         <v>443</v>
       </c>
-      <c r="C172" s="135" t="s">
+      <c r="C175" s="135" t="s">
         <v>415</v>
       </c>
-      <c r="D172" s="135" t="s">
+      <c r="D175" s="135" t="s">
         <v>415</v>
       </c>
-      <c r="E172" s="144"/>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A173" s="89" t="s">
+      <c r="E175" s="144"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176" s="89" t="s">
         <v>444</v>
       </c>
-      <c r="B173" s="90" t="s">
+      <c r="B176" s="90" t="s">
         <v>445</v>
       </c>
-      <c r="C173" s="135" t="s">
+      <c r="C176" s="135" t="s">
         <v>415</v>
       </c>
-      <c r="D173" s="135" t="s">
+      <c r="D176" s="135" t="s">
         <v>415</v>
       </c>
-      <c r="E173" s="144"/>
+      <c r="E176" s="144"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12966,7 +13650,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="A44" activeCellId="2" sqref="A42:XFD42 A43:XFD43 A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -32500,7 +33184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
@@ -32669,26 +33353,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6c854b04-c9c6-4391-adbe-2e73191270e7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="059b9c67-646b-4b4e-9ab1-2b1c805d0390">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AD6200282E8E804DB7E47654D11346C2" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="334b3f607926cb22599f187b4c015ce1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="059b9c67-646b-4b4e-9ab1-2b1c805d0390" xmlns:ns3="c05e7bd6-26a7-41a1-805c-893279a3732f" xmlns:ns4="6c854b04-c9c6-4391-adbe-2e73191270e7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0fe548b9ff7492f3109b4e0b4a8efc8f" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="059b9c67-646b-4b4e-9ab1-2b1c805d0390"/>
@@ -32948,26 +33612,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCA6965B-A23A-4F60-9CAE-00FD555BD4D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6c854b04-c9c6-4391-adbe-2e73191270e7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="059b9c67-646b-4b4e-9ab1-2b1c805d0390">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A2EA77E-CA9B-4563-9A5E-2F50B3C8BA13}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6c854b04-c9c6-4391-adbe-2e73191270e7"/>
-    <ds:schemaRef ds:uri="059b9c67-646b-4b4e-9ab1-2b1c805d0390"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FE51207-01AF-400E-9D05-58F426138751}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32985,4 +33650,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A2EA77E-CA9B-4563-9A5E-2F50B3C8BA13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6c854b04-c9c6-4391-adbe-2e73191270e7"/>
+    <ds:schemaRef ds:uri="059b9c67-646b-4b4e-9ab1-2b1c805d0390"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCA6965B-A23A-4F60-9CAE-00FD555BD4D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixing incorrect imperial unit in plant sheet
</commit_message>
<xml_diff>
--- a/data/static_tables/metric_structure.xlsx
+++ b/data/static_tables/metric_structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\eGrid\production_model\users\russelle\egrid\data\static_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3DB7BF-89D3-4A78-87EF-2D3443013D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095FAA27-2BEC-4AF5-A524-8BA1851BFEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10136,7 +10136,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E20"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -10414,8 +10414,8 @@
   <dimension ref="A1:IN176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G76" sqref="G76"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -12513,7 +12513,7 @@
         <v>34</v>
       </c>
       <c r="D101" s="130" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E101" s="144"/>
     </row>
@@ -33353,6 +33353,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6c854b04-c9c6-4391-adbe-2e73191270e7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="059b9c67-646b-4b4e-9ab1-2b1c805d0390">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AD6200282E8E804DB7E47654D11346C2" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="334b3f607926cb22599f187b4c015ce1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="059b9c67-646b-4b4e-9ab1-2b1c805d0390" xmlns:ns3="c05e7bd6-26a7-41a1-805c-893279a3732f" xmlns:ns4="6c854b04-c9c6-4391-adbe-2e73191270e7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0fe548b9ff7492f3109b4e0b4a8efc8f" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="059b9c67-646b-4b4e-9ab1-2b1c805d0390"/>
@@ -33612,27 +33632,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6c854b04-c9c6-4391-adbe-2e73191270e7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="059b9c67-646b-4b4e-9ab1-2b1c805d0390">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCA6965B-A23A-4F60-9CAE-00FD555BD4D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A2EA77E-CA9B-4563-9A5E-2F50B3C8BA13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6c854b04-c9c6-4391-adbe-2e73191270e7"/>
+    <ds:schemaRef ds:uri="059b9c67-646b-4b4e-9ab1-2b1c805d0390"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FE51207-01AF-400E-9D05-58F426138751}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33650,23 +33669,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A2EA77E-CA9B-4563-9A5E-2F50B3C8BA13}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6c854b04-c9c6-4391-adbe-2e73191270e7"/>
-    <ds:schemaRef ds:uri="059b9c67-646b-4b4e-9ab1-2b1c805d0390"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCA6965B-A23A-4F60-9CAE-00FD555BD4D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>